<commit_message>
Added FPGA to parts list and correct driver
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hong\Desktop\wave\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hong\Desktop\highway_wave\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FE23BF-D3B2-4B7E-AA9F-8730C1F8E158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C892FCFF-45D9-445C-A146-A0694B4F7959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{201324D8-1F9D-4E93-96FF-3B3C2E8BDCAF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Item</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Sound amp</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.us/item/3256804357132916.html?spm=a2g0o.detail.pcDetailTopMoreOtherSeller.4.2312gR10gR10R6&amp;gps-id=pcDetailTopMoreOtherSeller&amp;scm=1007.40196.439370.0&amp;scm_id=1007.40196.439370.0&amp;scm-url=1007.40196.439370.0&amp;pvid=bf9140d4-a701-43cf-87f1-e88529623557&amp;_t=gps-id:pcDetailTopMoreOtherSeller,scm-url:1007.40196.439370.0,pvid:bf9140d4-a701-43cf-87f1-e88529623557,tpp_buckets:668%232846%238109%231935&amp;pdp_ext_f=%7B%22order%22%3A%22-1%22%2C%22eval%22%3A%221%22%2C%22sceneId%22%3A%2230050%22%7D&amp;pdp_npi=4%40dis%21USD%2120.99%2112.59%21%21%2120.99%2112.59%21%402101c5b117499694560034258ea807%2112000029547617166%21rec%21US%21%21ABX&amp;utparam-url=scene%3ApcDetailTopMoreOtherSeller%7Cquery_from%3A</t>
   </si>
 </sst>
 </file>
@@ -538,7 +541,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D2" activeCellId="1" sqref="A2:A6 D2:D6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -576,6 +579,9 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
       <c r="D2" s="1">
         <v>10</v>
       </c>

</xml_diff>